<commit_message>
added risk list, and new iteration plan
</commit_message>
<xml_diff>
--- a/docs/project_management/risk list .xlsx
+++ b/docs/project_management/risk list .xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="93">
   <si>
     <t>Risk list SE04</t>
   </si>
@@ -29,6 +29,21 @@
   </si>
   <si>
     <t>Iteration 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Iteration 6 </t>
+  </si>
+  <si>
+    <t>Iteration 7</t>
+  </si>
+  <si>
+    <t>Iteration 8</t>
+  </si>
+  <si>
+    <t>Iteration 9</t>
+  </si>
+  <si>
+    <t>Iteration 10</t>
   </si>
   <si>
     <t>ID</t>
@@ -850,7 +865,7 @@
       <name val="Helvetica Neue"/>
     </font>
   </fonts>
-  <fills count="16">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -877,12 +892,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="16"/>
-        <bgColor auto="1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor indexed="17"/>
         <bgColor auto="1"/>
       </patternFill>
@@ -896,12 +905,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="19"/>
-        <bgColor auto="1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="20"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
@@ -925,6 +928,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor indexed="16"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor indexed="24"/>
         <bgColor auto="1"/>
       </patternFill>
@@ -941,8 +950,20 @@
         <bgColor auto="1"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="27"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="28"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="30">
+  <borders count="44">
     <border>
       <left/>
       <right/>
@@ -1029,6 +1050,36 @@
       <left style="thick">
         <color indexed="15"/>
       </left>
+      <right style="thick">
+        <color indexed="16"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="12"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="16"/>
+      </left>
+      <right style="thin">
+        <color indexed="12"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="12"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="15"/>
+      </left>
       <right style="thin">
         <color indexed="11"/>
       </right>
@@ -1097,6 +1148,36 @@
       </top>
       <bottom style="thin">
         <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="12"/>
+      </left>
+      <right style="thick">
+        <color indexed="16"/>
+      </right>
+      <top style="thin">
+        <color indexed="12"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="16"/>
+      </left>
+      <right style="thin">
+        <color indexed="12"/>
+      </right>
+      <top style="thin">
+        <color indexed="12"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="16"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1194,6 +1275,51 @@
       <left style="thin">
         <color indexed="12"/>
       </left>
+      <right style="thick">
+        <color indexed="16"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="12"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="16"/>
+      </left>
+      <right style="thin">
+        <color indexed="20"/>
+      </right>
+      <top style="thin">
+        <color indexed="16"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="20"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="20"/>
+      </left>
+      <right style="thick">
+        <color indexed="15"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="12"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="12"/>
+      </left>
       <right style="thin">
         <color indexed="11"/>
       </right>
@@ -1284,8 +1410,83 @@
       <left style="thin">
         <color indexed="12"/>
       </left>
+      <right style="thick">
+        <color indexed="16"/>
+      </right>
+      <top style="thin">
+        <color indexed="12"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="12"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="16"/>
+      </left>
+      <right style="thin">
+        <color indexed="20"/>
+      </right>
+      <top style="thin">
+        <color indexed="20"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="20"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="20"/>
+      </left>
+      <right style="thick">
+        <color indexed="15"/>
+      </right>
+      <top style="thin">
+        <color indexed="12"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="12"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="12"/>
+      </left>
       <right style="thin">
         <color indexed="11"/>
+      </right>
+      <top style="thin">
+        <color indexed="12"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="12"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="16"/>
+      </left>
+      <right style="thin">
+        <color indexed="12"/>
+      </right>
+      <top style="thin">
+        <color indexed="20"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="12"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="16"/>
+      </left>
+      <right style="thin">
+        <color indexed="12"/>
       </right>
       <top style="thin">
         <color indexed="12"/>
@@ -1374,6 +1575,36 @@
       <left style="thin">
         <color indexed="12"/>
       </left>
+      <right style="thick">
+        <color indexed="16"/>
+      </right>
+      <top style="thin">
+        <color indexed="12"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="16"/>
+      </left>
+      <right style="thin">
+        <color indexed="12"/>
+      </right>
+      <top style="thin">
+        <color indexed="12"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="12"/>
+      </left>
       <right style="thin">
         <color indexed="11"/>
       </right>
@@ -1391,7 +1622,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="95">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1431,16 +1662,10 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="4" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1449,85 +1674,55 @@
     <xf numFmtId="49" fontId="3" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="59" fontId="7" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="7" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="4" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="6" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="59" fontId="7" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" indent="1" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="7" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="7" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="5" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center" indent="3" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="6" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="8" fillId="6" borderId="20" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center" indent="3" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="8" borderId="19" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="7" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center" indent="3" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="59" fontId="7" fillId="8" borderId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="8" borderId="20" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="20" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="4" borderId="20" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" indent="1" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="8" borderId="20" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="9" borderId="21" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center" indent="3" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="5" borderId="22" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center" indent="3" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="21" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="23" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="59" fontId="7" borderId="19" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" borderId="20" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" borderId="20" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="10" borderId="21" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center" indent="3" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="9" borderId="22" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="8" fillId="7" borderId="20" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center" indent="3" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" borderId="21" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1536,67 +1731,181 @@
     <xf numFmtId="49" fontId="8" fillId="6" borderId="22" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center" indent="3" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="7" borderId="22" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center" indent="3" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="11" borderId="22" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center" indent="3" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" borderId="23" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="11" borderId="21" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="20" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="19" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="24" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" borderId="25" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="59" fontId="7" fillId="9" borderId="26" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="9" borderId="27" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="27" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="27" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" indent="1" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="9" borderId="27" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="10" borderId="28" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center" indent="3" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="12" borderId="21" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="8" fillId="5" borderId="29" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center" indent="3" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="13" borderId="22" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="28" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="30" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="5" borderId="31" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center" indent="3" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="8" borderId="20" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="32" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="29" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="28" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="33" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="59" fontId="7" borderId="26" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" borderId="27" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" borderId="27" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="11" borderId="28" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center" indent="3" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="10" borderId="29" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center" indent="3" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" borderId="28" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="6" borderId="29" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center" indent="3" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="7" borderId="29" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center" indent="3" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="12" borderId="29" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center" indent="3" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" borderId="30" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="10" borderId="31" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center" indent="3" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" borderId="32" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="12" borderId="28" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center" indent="3" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="7" borderId="34" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center" indent="3" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="13" borderId="28" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center" indent="3" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="14" borderId="29" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center" indent="3" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="6" borderId="35" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center" indent="3" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="9" borderId="27" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="4" borderId="20" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="8" fillId="10" borderId="35" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center" indent="3" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="5" borderId="35" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center" indent="3" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="12" borderId="35" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center" indent="3" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="27" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="14" borderId="22" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="8" fillId="7" borderId="35" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center" indent="3" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="15" borderId="22" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="8" fillId="15" borderId="29" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center" indent="3" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" borderId="24" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="8" fillId="16" borderId="29" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center" indent="3" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" borderId="36" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="59" fontId="7" fillId="8" borderId="25" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="59" fontId="7" fillId="9" borderId="37" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="8" borderId="26" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="7" fillId="9" borderId="38" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="26" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="38" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="4" borderId="26" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="38" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" indent="1" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="8" borderId="26" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="7" fillId="9" borderId="38" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="11" borderId="27" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="2" fillId="12" borderId="39" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center" indent="3" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="15" borderId="28" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="8" fillId="16" borderId="40" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center" indent="3" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="27" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="39" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="6" borderId="28" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="8" fillId="6" borderId="40" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center" indent="3" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="29" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="41" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="16" borderId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center" indent="3" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="40" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="39" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="43" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1623,12 +1932,14 @@
       <rgbColor rgb="ff004c7f"/>
       <rgbColor rgb="ff017a75"/>
       <rgbColor rgb="ff6c6c6c"/>
+      <rgbColor rgb="ffee210c"/>
       <rgbColor rgb="ff1cb000"/>
       <rgbColor rgb="fff8b900"/>
       <rgbColor rgb="ff004e05"/>
+      <rgbColor rgb="fff69085"/>
+      <rgbColor rgb="ff00a1fe"/>
       <rgbColor rgb="ffa9a9a9"/>
       <rgbColor rgb="ffd65e01"/>
-      <rgbColor rgb="ffee210c"/>
       <rgbColor rgb="ff017000"/>
       <rgbColor rgb="fffae232"/>
       <rgbColor rgb="ff60d735"/>
@@ -2662,7 +2973,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A2:Q21"/>
+  <dimension ref="A2:AA21"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
       <pane topLeftCell="B4" xSplit="1" ySplit="3" activePane="bottomRight" state="frozen"/>
@@ -2683,9 +2994,20 @@
     <col min="12" max="12" width="16.3516" style="1" customWidth="1"/>
     <col min="13" max="13" width="5.67188" style="1" customWidth="1"/>
     <col min="14" max="14" width="16.3516" style="1" customWidth="1"/>
-    <col min="15" max="15" width="5.67188" style="1" customWidth="1"/>
-    <col min="16" max="17" width="16.3516" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="16.3516" style="1" customWidth="1"/>
+    <col min="15" max="15" width="6.04688" style="1" customWidth="1"/>
+    <col min="16" max="16" width="16.3516" style="1" customWidth="1"/>
+    <col min="17" max="17" width="6.04688" style="1" customWidth="1"/>
+    <col min="18" max="18" width="16.3516" style="1" customWidth="1"/>
+    <col min="19" max="19" width="6.04688" style="1" customWidth="1"/>
+    <col min="20" max="20" width="16.3516" style="1" customWidth="1"/>
+    <col min="21" max="21" width="6.04688" style="1" customWidth="1"/>
+    <col min="22" max="22" width="16.3516" style="1" customWidth="1"/>
+    <col min="23" max="23" width="6.04688" style="1" customWidth="1"/>
+    <col min="24" max="24" width="16.4688" style="1" customWidth="1"/>
+    <col min="25" max="25" width="6" style="1" customWidth="1"/>
+    <col min="26" max="26" width="16.4219" style="1" customWidth="1"/>
+    <col min="27" max="27" width="5.92188" style="1" customWidth="1"/>
+    <col min="28" max="16384" width="16.3516" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="25.65" customHeight="1">
@@ -2708,6 +3030,16 @@
       <c r="O1" s="2"/>
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
+      <c r="U1" s="2"/>
+      <c r="V1" s="2"/>
+      <c r="W1" s="2"/>
+      <c r="X1" s="2"/>
+      <c r="Y1" s="2"/>
+      <c r="Z1" s="2"/>
+      <c r="AA1" s="2"/>
     </row>
     <row r="2" ht="22.5" customHeight="1">
       <c r="A2" s="3"/>
@@ -2737,1112 +3069,1437 @@
         <v>5</v>
       </c>
       <c r="Q2" s="12"/>
+      <c r="R2" t="s" s="13">
+        <v>6</v>
+      </c>
+      <c r="S2" s="9"/>
+      <c r="T2" t="s" s="8">
+        <v>7</v>
+      </c>
+      <c r="U2" s="9"/>
+      <c r="V2" t="s" s="10">
+        <v>8</v>
+      </c>
+      <c r="W2" s="11"/>
+      <c r="X2" t="s" s="10">
+        <v>9</v>
+      </c>
+      <c r="Y2" s="11"/>
+      <c r="Z2" t="s" s="10">
+        <v>10</v>
+      </c>
+      <c r="AA2" s="14"/>
     </row>
     <row r="3" ht="20.45" customHeight="1">
-      <c r="A3" t="s" s="13">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s" s="14">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s" s="14">
-        <v>8</v>
-      </c>
-      <c r="D3" t="s" s="15">
-        <v>9</v>
-      </c>
-      <c r="E3" t="s" s="16">
-        <v>10</v>
-      </c>
-      <c r="F3" t="s" s="14">
+      <c r="A3" t="s" s="15">
         <v>11</v>
       </c>
-      <c r="G3" t="s" s="17">
+      <c r="B3" t="s" s="16">
         <v>12</v>
       </c>
-      <c r="H3" t="s" s="18">
+      <c r="C3" t="s" s="16">
         <v>13</v>
       </c>
-      <c r="I3" t="s" s="17">
+      <c r="D3" t="s" s="17">
         <v>14</v>
       </c>
-      <c r="J3" t="s" s="18">
-        <v>13</v>
-      </c>
-      <c r="K3" t="s" s="17">
-        <v>14</v>
-      </c>
-      <c r="L3" t="s" s="18">
-        <v>13</v>
-      </c>
-      <c r="M3" t="s" s="17">
-        <v>14</v>
-      </c>
-      <c r="N3" t="s" s="18">
-        <v>13</v>
-      </c>
-      <c r="O3" t="s" s="17">
-        <v>14</v>
-      </c>
-      <c r="P3" t="s" s="18">
-        <v>13</v>
-      </c>
-      <c r="Q3" t="s" s="19">
-        <v>14</v>
+      <c r="E3" t="s" s="18">
+        <v>15</v>
+      </c>
+      <c r="F3" t="s" s="16">
+        <v>16</v>
+      </c>
+      <c r="G3" t="s" s="19">
+        <v>17</v>
+      </c>
+      <c r="H3" t="s" s="20">
+        <v>18</v>
+      </c>
+      <c r="I3" t="s" s="19">
+        <v>19</v>
+      </c>
+      <c r="J3" t="s" s="20">
+        <v>18</v>
+      </c>
+      <c r="K3" t="s" s="19">
+        <v>19</v>
+      </c>
+      <c r="L3" t="s" s="20">
+        <v>18</v>
+      </c>
+      <c r="M3" t="s" s="19">
+        <v>19</v>
+      </c>
+      <c r="N3" t="s" s="20">
+        <v>18</v>
+      </c>
+      <c r="O3" t="s" s="19">
+        <v>19</v>
+      </c>
+      <c r="P3" t="s" s="20">
+        <v>18</v>
+      </c>
+      <c r="Q3" t="s" s="21">
+        <v>19</v>
+      </c>
+      <c r="R3" t="s" s="22">
+        <v>18</v>
+      </c>
+      <c r="S3" t="s" s="19">
+        <v>19</v>
+      </c>
+      <c r="T3" t="s" s="20">
+        <v>18</v>
+      </c>
+      <c r="U3" t="s" s="19">
+        <v>19</v>
+      </c>
+      <c r="V3" t="s" s="20">
+        <v>18</v>
+      </c>
+      <c r="W3" t="s" s="19">
+        <v>19</v>
+      </c>
+      <c r="X3" t="s" s="20">
+        <v>18</v>
+      </c>
+      <c r="Y3" t="s" s="19">
+        <v>19</v>
+      </c>
+      <c r="Z3" t="s" s="20">
+        <v>18</v>
+      </c>
+      <c r="AA3" t="s" s="23">
+        <v>19</v>
       </c>
     </row>
     <row r="4" ht="140.45" customHeight="1">
-      <c r="A4" s="20">
+      <c r="A4" s="24">
         <v>1</v>
       </c>
-      <c r="B4" s="21">
+      <c r="B4" s="25">
         <v>45268</v>
       </c>
-      <c r="C4" t="s" s="22">
-        <v>15</v>
-      </c>
-      <c r="D4" t="s" s="23">
-        <v>16</v>
-      </c>
-      <c r="E4" t="s" s="24">
-        <v>17</v>
-      </c>
-      <c r="F4" t="s" s="25">
-        <v>18</v>
-      </c>
-      <c r="G4" t="s" s="26">
-        <v>19</v>
-      </c>
-      <c r="H4" t="s" s="27">
+      <c r="C4" t="s" s="26">
         <v>20</v>
       </c>
-      <c r="I4" s="28">
+      <c r="D4" t="s" s="27">
+        <v>21</v>
+      </c>
+      <c r="E4" t="s" s="28">
+        <v>22</v>
+      </c>
+      <c r="F4" t="s" s="29">
+        <v>23</v>
+      </c>
+      <c r="G4" t="s" s="30">
+        <v>24</v>
+      </c>
+      <c r="H4" t="s" s="31">
+        <v>25</v>
+      </c>
+      <c r="I4" s="32">
         <f>G4*H4</f>
         <v>0.4</v>
       </c>
-      <c r="J4" t="s" s="29">
-        <v>21</v>
-      </c>
-      <c r="K4" s="28">
+      <c r="J4" t="s" s="33">
+        <v>26</v>
+      </c>
+      <c r="K4" s="32">
         <f>J4*G4</f>
         <v>0.3</v>
       </c>
-      <c r="L4" t="s" s="29">
-        <v>21</v>
-      </c>
-      <c r="M4" s="28">
+      <c r="L4" t="s" s="33">
+        <v>26</v>
+      </c>
+      <c r="M4" s="32">
         <f>G4*L4</f>
         <v>0.3</v>
       </c>
-      <c r="N4" t="s" s="29">
-        <v>21</v>
-      </c>
-      <c r="O4" s="28">
+      <c r="N4" t="s" s="33">
+        <v>26</v>
+      </c>
+      <c r="O4" s="32">
         <f>N4*G4</f>
         <v>0.3</v>
       </c>
-      <c r="P4" t="s" s="29">
-        <v>21</v>
-      </c>
-      <c r="Q4" s="30">
+      <c r="P4" t="s" s="33">
+        <v>26</v>
+      </c>
+      <c r="Q4" s="34">
         <f>P4*G4</f>
         <v>0.3</v>
       </c>
+      <c r="R4" t="s" s="35">
+        <v>25</v>
+      </c>
+      <c r="S4" s="36">
+        <f>G4*R4</f>
+        <v>0.4</v>
+      </c>
+      <c r="T4" s="37"/>
+      <c r="U4" s="38"/>
+      <c r="V4" s="37"/>
+      <c r="W4" s="38"/>
+      <c r="X4" s="37"/>
+      <c r="Y4" s="38"/>
+      <c r="Z4" s="37"/>
+      <c r="AA4" s="39"/>
     </row>
     <row r="5" ht="128.2" customHeight="1">
-      <c r="A5" s="31">
+      <c r="A5" s="40">
         <v>2</v>
       </c>
-      <c r="B5" s="32">
+      <c r="B5" s="41">
         <v>45268</v>
       </c>
-      <c r="C5" t="s" s="33">
-        <v>22</v>
-      </c>
-      <c r="D5" t="s" s="34">
-        <v>23</v>
-      </c>
-      <c r="E5" t="s" s="35">
-        <v>24</v>
-      </c>
-      <c r="F5" t="s" s="36">
-        <v>25</v>
-      </c>
-      <c r="G5" t="s" s="37">
-        <v>26</v>
-      </c>
-      <c r="H5" t="s" s="38">
+      <c r="C5" t="s" s="42">
         <v>27</v>
       </c>
-      <c r="I5" s="39">
+      <c r="D5" t="s" s="43">
+        <v>28</v>
+      </c>
+      <c r="E5" t="s" s="44">
+        <v>29</v>
+      </c>
+      <c r="F5" t="s" s="45">
+        <v>30</v>
+      </c>
+      <c r="G5" t="s" s="46">
+        <v>31</v>
+      </c>
+      <c r="H5" t="s" s="47">
+        <v>32</v>
+      </c>
+      <c r="I5" s="48">
         <f>G5*H5</f>
         <v>0.4</v>
       </c>
-      <c r="J5" t="s" s="38">
-        <v>27</v>
-      </c>
-      <c r="K5" s="39">
+      <c r="J5" t="s" s="47">
+        <v>32</v>
+      </c>
+      <c r="K5" s="48">
         <f>J5*G5</f>
         <v>0.4</v>
       </c>
-      <c r="L5" t="s" s="38">
-        <v>27</v>
-      </c>
-      <c r="M5" s="39">
+      <c r="L5" t="s" s="47">
+        <v>32</v>
+      </c>
+      <c r="M5" s="48">
         <f>G5*L5</f>
         <v>0.4</v>
       </c>
-      <c r="N5" t="s" s="38">
-        <v>27</v>
-      </c>
-      <c r="O5" s="39">
+      <c r="N5" t="s" s="47">
+        <v>32</v>
+      </c>
+      <c r="O5" s="48">
         <f>N5*G5</f>
         <v>0.4</v>
       </c>
-      <c r="P5" t="s" s="38">
-        <v>27</v>
-      </c>
-      <c r="Q5" s="40">
+      <c r="P5" t="s" s="47">
+        <v>32</v>
+      </c>
+      <c r="Q5" s="49">
         <f>P5*G5</f>
         <v>0.4</v>
       </c>
+      <c r="R5" t="s" s="50">
+        <v>32</v>
+      </c>
+      <c r="S5" s="51">
+        <f>G5*R5</f>
+        <v>0.4</v>
+      </c>
+      <c r="T5" s="52"/>
+      <c r="U5" s="53"/>
+      <c r="V5" s="52"/>
+      <c r="W5" s="53"/>
+      <c r="X5" s="52"/>
+      <c r="Y5" s="53"/>
+      <c r="Z5" s="52"/>
+      <c r="AA5" s="54"/>
     </row>
     <row r="6" ht="80.2" customHeight="1">
-      <c r="A6" s="31">
+      <c r="A6" s="40">
         <v>3</v>
       </c>
-      <c r="B6" s="41">
+      <c r="B6" s="55">
         <v>45268</v>
       </c>
-      <c r="C6" t="s" s="42">
-        <v>28</v>
-      </c>
-      <c r="D6" t="s" s="34">
-        <v>29</v>
-      </c>
-      <c r="E6" t="s" s="35">
+      <c r="C6" t="s" s="56">
+        <v>33</v>
+      </c>
+      <c r="D6" t="s" s="43">
+        <v>34</v>
+      </c>
+      <c r="E6" t="s" s="44">
+        <v>35</v>
+      </c>
+      <c r="F6" t="s" s="57">
         <v>30</v>
       </c>
-      <c r="F6" t="s" s="43">
-        <v>25</v>
-      </c>
-      <c r="G6" t="s" s="44">
-        <v>31</v>
-      </c>
-      <c r="H6" t="s" s="45">
-        <v>32</v>
-      </c>
-      <c r="I6" s="46">
+      <c r="G6" t="s" s="58">
+        <v>36</v>
+      </c>
+      <c r="H6" t="s" s="59">
+        <v>37</v>
+      </c>
+      <c r="I6" s="60">
         <f>G6*H6</f>
         <v>3</v>
       </c>
-      <c r="J6" t="s" s="47">
-        <v>20</v>
-      </c>
-      <c r="K6" s="46">
+      <c r="J6" t="s" s="61">
+        <v>25</v>
+      </c>
+      <c r="K6" s="60">
         <f>G6*J6</f>
         <v>2</v>
       </c>
-      <c r="L6" t="s" s="48">
-        <v>21</v>
-      </c>
-      <c r="M6" s="46">
+      <c r="L6" t="s" s="62">
+        <v>26</v>
+      </c>
+      <c r="M6" s="60">
         <f>G6*L6</f>
         <v>1.5</v>
       </c>
-      <c r="N6" t="s" s="48">
-        <v>21</v>
-      </c>
-      <c r="O6" s="46">
+      <c r="N6" t="s" s="62">
+        <v>26</v>
+      </c>
+      <c r="O6" s="60">
         <f>N6*G6</f>
         <v>1.5</v>
       </c>
-      <c r="P6" t="s" s="49">
-        <v>33</v>
-      </c>
-      <c r="Q6" s="50">
+      <c r="P6" t="s" s="63">
+        <v>38</v>
+      </c>
+      <c r="Q6" s="64">
         <f>P6*G6</f>
         <v>1</v>
       </c>
+      <c r="R6" t="s" s="65">
+        <v>37</v>
+      </c>
+      <c r="S6" s="66">
+        <f>G6*R6</f>
+        <v>3</v>
+      </c>
+      <c r="T6" s="52"/>
+      <c r="U6" s="53"/>
+      <c r="V6" s="52"/>
+      <c r="W6" s="53"/>
+      <c r="X6" s="52"/>
+      <c r="Y6" s="53"/>
+      <c r="Z6" s="52"/>
+      <c r="AA6" s="54"/>
     </row>
     <row r="7" ht="92.2" customHeight="1">
-      <c r="A7" s="31">
+      <c r="A7" s="40">
         <v>4</v>
       </c>
-      <c r="B7" s="32">
+      <c r="B7" s="41">
         <v>45270</v>
       </c>
-      <c r="C7" t="s" s="33">
-        <v>34</v>
-      </c>
-      <c r="D7" t="s" s="34">
-        <v>35</v>
-      </c>
-      <c r="E7" t="s" s="35">
-        <v>36</v>
-      </c>
-      <c r="F7" t="s" s="36">
-        <v>37</v>
-      </c>
-      <c r="G7" t="s" s="51">
+      <c r="C7" t="s" s="42">
+        <v>39</v>
+      </c>
+      <c r="D7" t="s" s="43">
+        <v>40</v>
+      </c>
+      <c r="E7" t="s" s="44">
+        <v>41</v>
+      </c>
+      <c r="F7" t="s" s="45">
+        <v>42</v>
+      </c>
+      <c r="G7" t="s" s="67">
+        <v>43</v>
+      </c>
+      <c r="H7" t="s" s="63">
         <v>38</v>
       </c>
-      <c r="H7" t="s" s="49">
-        <v>33</v>
-      </c>
-      <c r="I7" s="39">
+      <c r="I7" s="48">
         <f>G7*H7</f>
         <v>0.4</v>
       </c>
-      <c r="J7" t="s" s="48">
-        <v>21</v>
-      </c>
-      <c r="K7" s="39">
+      <c r="J7" t="s" s="62">
+        <v>26</v>
+      </c>
+      <c r="K7" s="48">
         <f>G7*J7</f>
         <v>0.6</v>
       </c>
-      <c r="L7" t="s" s="48">
-        <v>21</v>
-      </c>
-      <c r="M7" s="39">
+      <c r="L7" t="s" s="62">
+        <v>26</v>
+      </c>
+      <c r="M7" s="48">
         <f>G7*L7</f>
         <v>0.6</v>
       </c>
-      <c r="N7" t="s" s="47">
-        <v>20</v>
-      </c>
-      <c r="O7" s="39">
+      <c r="N7" t="s" s="61">
+        <v>25</v>
+      </c>
+      <c r="O7" s="48">
         <f>N7*G7</f>
         <v>0.8</v>
       </c>
-      <c r="P7" t="s" s="48">
-        <v>21</v>
-      </c>
-      <c r="Q7" s="40">
+      <c r="P7" t="s" s="62">
+        <v>26</v>
+      </c>
+      <c r="Q7" s="49">
         <f>P7*G7</f>
         <v>0.6</v>
       </c>
+      <c r="R7" t="s" s="68">
+        <v>26</v>
+      </c>
+      <c r="S7" s="48">
+        <f>G7*R7</f>
+        <v>0.6</v>
+      </c>
+      <c r="T7" s="52"/>
+      <c r="U7" s="53"/>
+      <c r="V7" s="52"/>
+      <c r="W7" s="53"/>
+      <c r="X7" s="52"/>
+      <c r="Y7" s="53"/>
+      <c r="Z7" s="52"/>
+      <c r="AA7" s="54"/>
     </row>
     <row r="8" ht="95.1" customHeight="1">
-      <c r="A8" s="31">
+      <c r="A8" s="40">
         <v>5</v>
       </c>
-      <c r="B8" s="41">
+      <c r="B8" s="55">
         <v>45270</v>
       </c>
-      <c r="C8" t="s" s="42">
-        <v>39</v>
-      </c>
-      <c r="D8" t="s" s="34">
-        <v>40</v>
-      </c>
-      <c r="E8" t="s" s="35">
-        <v>41</v>
-      </c>
-      <c r="F8" t="s" s="43">
-        <v>42</v>
-      </c>
-      <c r="G8" t="s" s="52">
-        <v>43</v>
-      </c>
-      <c r="H8" t="s" s="53">
+      <c r="C8" t="s" s="56">
         <v>44</v>
       </c>
-      <c r="I8" s="46">
+      <c r="D8" t="s" s="43">
+        <v>45</v>
+      </c>
+      <c r="E8" t="s" s="44">
+        <v>46</v>
+      </c>
+      <c r="F8" t="s" s="57">
+        <v>47</v>
+      </c>
+      <c r="G8" t="s" s="69">
+        <v>48</v>
+      </c>
+      <c r="H8" t="s" s="70">
+        <v>49</v>
+      </c>
+      <c r="I8" s="60">
         <f>G8*H8</f>
         <v>0</v>
       </c>
-      <c r="J8" t="s" s="53">
-        <v>44</v>
-      </c>
-      <c r="K8" s="46">
+      <c r="J8" t="s" s="70">
+        <v>49</v>
+      </c>
+      <c r="K8" s="60">
         <f>G8*J8</f>
         <v>0</v>
       </c>
-      <c r="L8" t="s" s="53">
-        <v>44</v>
-      </c>
-      <c r="M8" s="46">
+      <c r="L8" t="s" s="70">
+        <v>49</v>
+      </c>
+      <c r="M8" s="60">
         <f>G8*L8</f>
         <v>0</v>
       </c>
-      <c r="N8" t="s" s="47">
-        <v>20</v>
-      </c>
-      <c r="O8" s="46">
+      <c r="N8" t="s" s="61">
+        <v>25</v>
+      </c>
+      <c r="O8" s="60">
         <f>N8*G8</f>
         <v>1.2</v>
       </c>
-      <c r="P8" t="s" s="47">
-        <v>20</v>
-      </c>
-      <c r="Q8" s="50">
+      <c r="P8" t="s" s="61">
+        <v>25</v>
+      </c>
+      <c r="Q8" s="64">
         <f>P8*G8</f>
         <v>1.2</v>
       </c>
+      <c r="R8" t="s" s="71">
+        <v>25</v>
+      </c>
+      <c r="S8" s="60">
+        <f>G8*R8</f>
+        <v>1.2</v>
+      </c>
+      <c r="T8" s="52"/>
+      <c r="U8" s="53"/>
+      <c r="V8" s="52"/>
+      <c r="W8" s="53"/>
+      <c r="X8" s="52"/>
+      <c r="Y8" s="53"/>
+      <c r="Z8" s="52"/>
+      <c r="AA8" s="54"/>
     </row>
     <row r="9" ht="83.1" customHeight="1">
-      <c r="A9" s="31">
+      <c r="A9" s="40">
         <v>6</v>
       </c>
-      <c r="B9" s="32">
+      <c r="B9" s="41">
         <v>45270</v>
       </c>
-      <c r="C9" t="s" s="54">
-        <v>45</v>
-      </c>
-      <c r="D9" t="s" s="34">
-        <v>46</v>
-      </c>
-      <c r="E9" t="s" s="35">
-        <v>47</v>
-      </c>
-      <c r="F9" t="s" s="36">
-        <v>48</v>
-      </c>
-      <c r="G9" t="s" s="51">
-        <v>38</v>
-      </c>
-      <c r="H9" t="s" s="53">
-        <v>44</v>
-      </c>
-      <c r="I9" s="39">
+      <c r="C9" t="s" s="72">
+        <v>50</v>
+      </c>
+      <c r="D9" t="s" s="43">
+        <v>51</v>
+      </c>
+      <c r="E9" t="s" s="44">
+        <v>52</v>
+      </c>
+      <c r="F9" t="s" s="45">
+        <v>53</v>
+      </c>
+      <c r="G9" t="s" s="67">
+        <v>43</v>
+      </c>
+      <c r="H9" t="s" s="70">
+        <v>49</v>
+      </c>
+      <c r="I9" s="48">
         <f>G9*H9</f>
         <v>0</v>
       </c>
-      <c r="J9" t="s" s="53">
-        <v>44</v>
-      </c>
-      <c r="K9" s="39">
+      <c r="J9" t="s" s="70">
+        <v>49</v>
+      </c>
+      <c r="K9" s="48">
         <f>G9*J9</f>
         <v>0</v>
       </c>
-      <c r="L9" t="s" s="53">
-        <v>44</v>
-      </c>
-      <c r="M9" s="39">
+      <c r="L9" t="s" s="70">
+        <v>49</v>
+      </c>
+      <c r="M9" s="48">
         <f>G9*L9</f>
         <v>0</v>
       </c>
-      <c r="N9" t="s" s="45">
-        <v>32</v>
-      </c>
-      <c r="O9" s="39">
+      <c r="N9" t="s" s="59">
+        <v>37</v>
+      </c>
+      <c r="O9" s="48">
         <f>N9*G9</f>
         <v>1.2</v>
       </c>
-      <c r="P9" t="s" s="45">
-        <v>32</v>
-      </c>
-      <c r="Q9" s="40">
+      <c r="P9" t="s" s="59">
+        <v>37</v>
+      </c>
+      <c r="Q9" s="49">
         <f>P9*G9</f>
         <v>1.2</v>
       </c>
+      <c r="R9" t="s" s="73">
+        <v>37</v>
+      </c>
+      <c r="S9" s="48">
+        <f>G9*R9</f>
+        <v>1.2</v>
+      </c>
+      <c r="T9" s="52"/>
+      <c r="U9" s="53"/>
+      <c r="V9" s="52"/>
+      <c r="W9" s="53"/>
+      <c r="X9" s="52"/>
+      <c r="Y9" s="53"/>
+      <c r="Z9" s="52"/>
+      <c r="AA9" s="54"/>
     </row>
     <row r="10" ht="68.2" customHeight="1">
-      <c r="A10" s="31">
+      <c r="A10" s="40">
         <v>7</v>
       </c>
-      <c r="B10" s="41">
+      <c r="B10" s="55">
         <v>45270</v>
       </c>
-      <c r="C10" t="s" s="42">
+      <c r="C10" t="s" s="56">
+        <v>54</v>
+      </c>
+      <c r="D10" t="s" s="43">
+        <v>55</v>
+      </c>
+      <c r="E10" t="s" s="44">
+        <v>56</v>
+      </c>
+      <c r="F10" t="s" s="57">
+        <v>30</v>
+      </c>
+      <c r="G10" t="s" s="69">
+        <v>48</v>
+      </c>
+      <c r="H10" t="s" s="70">
         <v>49</v>
       </c>
-      <c r="D10" t="s" s="34">
-        <v>50</v>
-      </c>
-      <c r="E10" t="s" s="35">
-        <v>51</v>
-      </c>
-      <c r="F10" t="s" s="43">
-        <v>25</v>
-      </c>
-      <c r="G10" t="s" s="52">
-        <v>43</v>
-      </c>
-      <c r="H10" t="s" s="53">
-        <v>44</v>
-      </c>
-      <c r="I10" s="46">
+      <c r="I10" s="60">
         <f>G10*H10</f>
         <v>0</v>
       </c>
-      <c r="J10" t="s" s="53">
-        <v>44</v>
-      </c>
-      <c r="K10" s="46">
+      <c r="J10" t="s" s="70">
+        <v>49</v>
+      </c>
+      <c r="K10" s="60">
         <f>G10*J10</f>
         <v>0</v>
       </c>
-      <c r="L10" t="s" s="53">
-        <v>44</v>
-      </c>
-      <c r="M10" s="46">
+      <c r="L10" t="s" s="70">
+        <v>49</v>
+      </c>
+      <c r="M10" s="60">
         <f>G10*L10</f>
         <v>0</v>
       </c>
-      <c r="N10" t="s" s="38">
-        <v>27</v>
-      </c>
-      <c r="O10" s="46">
+      <c r="N10" t="s" s="47">
+        <v>32</v>
+      </c>
+      <c r="O10" s="60">
         <f>N10*G10</f>
         <v>0.3</v>
       </c>
-      <c r="P10" t="s" s="38">
-        <v>27</v>
-      </c>
-      <c r="Q10" s="50">
+      <c r="P10" t="s" s="47">
+        <v>32</v>
+      </c>
+      <c r="Q10" s="64">
         <f>P10*G10</f>
         <v>0.3</v>
       </c>
+      <c r="R10" t="s" s="74">
+        <v>32</v>
+      </c>
+      <c r="S10" s="60">
+        <f>G10*R10</f>
+        <v>0.3</v>
+      </c>
+      <c r="T10" s="52"/>
+      <c r="U10" s="53"/>
+      <c r="V10" s="52"/>
+      <c r="W10" s="53"/>
+      <c r="X10" s="52"/>
+      <c r="Y10" s="53"/>
+      <c r="Z10" s="52"/>
+      <c r="AA10" s="54"/>
     </row>
     <row r="11" ht="128.2" customHeight="1">
-      <c r="A11" s="31">
+      <c r="A11" s="40">
         <v>8</v>
       </c>
-      <c r="B11" s="32">
+      <c r="B11" s="41">
         <v>45270</v>
       </c>
-      <c r="C11" t="s" s="33">
-        <v>52</v>
-      </c>
-      <c r="D11" t="s" s="34">
-        <v>53</v>
-      </c>
-      <c r="E11" t="s" s="35">
-        <v>54</v>
-      </c>
-      <c r="F11" t="s" s="36">
-        <v>42</v>
-      </c>
-      <c r="G11" t="s" s="51">
-        <v>38</v>
-      </c>
-      <c r="H11" t="s" s="53">
-        <v>44</v>
-      </c>
-      <c r="I11" s="39">
+      <c r="C11" t="s" s="42">
+        <v>57</v>
+      </c>
+      <c r="D11" t="s" s="43">
+        <v>58</v>
+      </c>
+      <c r="E11" t="s" s="44">
+        <v>59</v>
+      </c>
+      <c r="F11" t="s" s="45">
+        <v>47</v>
+      </c>
+      <c r="G11" t="s" s="67">
+        <v>43</v>
+      </c>
+      <c r="H11" t="s" s="70">
+        <v>49</v>
+      </c>
+      <c r="I11" s="48">
         <f>G11*H11</f>
         <v>0</v>
       </c>
-      <c r="J11" t="s" s="53">
-        <v>44</v>
-      </c>
-      <c r="K11" s="39">
+      <c r="J11" t="s" s="70">
+        <v>49</v>
+      </c>
+      <c r="K11" s="48">
         <f>G11*J11</f>
         <v>0</v>
       </c>
-      <c r="L11" t="s" s="53">
-        <v>44</v>
-      </c>
-      <c r="M11" s="39">
+      <c r="L11" t="s" s="70">
+        <v>49</v>
+      </c>
+      <c r="M11" s="48">
         <f>G11*L11</f>
         <v>0</v>
       </c>
-      <c r="N11" t="s" s="38">
-        <v>27</v>
-      </c>
-      <c r="O11" s="39">
+      <c r="N11" t="s" s="47">
+        <v>32</v>
+      </c>
+      <c r="O11" s="48">
         <f>N11*G11</f>
         <v>0.2</v>
       </c>
-      <c r="P11" t="s" s="38">
-        <v>27</v>
-      </c>
-      <c r="Q11" s="40">
+      <c r="P11" t="s" s="47">
+        <v>32</v>
+      </c>
+      <c r="Q11" s="49">
         <f>P11*G11</f>
         <v>0.2</v>
       </c>
+      <c r="R11" t="s" s="75">
+        <v>38</v>
+      </c>
+      <c r="S11" s="48">
+        <f>G11*R11</f>
+        <v>0.4</v>
+      </c>
+      <c r="T11" s="52"/>
+      <c r="U11" s="53"/>
+      <c r="V11" s="52"/>
+      <c r="W11" s="53"/>
+      <c r="X11" s="52"/>
+      <c r="Y11" s="53"/>
+      <c r="Z11" s="52"/>
+      <c r="AA11" s="54"/>
     </row>
     <row r="12" ht="92.2" customHeight="1">
-      <c r="A12" s="31">
+      <c r="A12" s="40">
         <v>9</v>
       </c>
-      <c r="B12" s="41">
+      <c r="B12" s="55">
         <v>45270</v>
       </c>
-      <c r="C12" t="s" s="42">
-        <v>55</v>
-      </c>
-      <c r="D12" t="s" s="34">
-        <v>56</v>
-      </c>
-      <c r="E12" t="s" s="35">
-        <v>57</v>
-      </c>
-      <c r="F12" t="s" s="43">
-        <v>37</v>
-      </c>
-      <c r="G12" t="s" s="44">
-        <v>31</v>
-      </c>
-      <c r="H12" t="s" s="49">
-        <v>58</v>
-      </c>
-      <c r="I12" s="46">
+      <c r="C12" t="s" s="56">
+        <v>60</v>
+      </c>
+      <c r="D12" t="s" s="43">
+        <v>61</v>
+      </c>
+      <c r="E12" t="s" s="44">
+        <v>62</v>
+      </c>
+      <c r="F12" t="s" s="57">
+        <v>42</v>
+      </c>
+      <c r="G12" t="s" s="58">
+        <v>36</v>
+      </c>
+      <c r="H12" t="s" s="63">
+        <v>63</v>
+      </c>
+      <c r="I12" s="60">
         <f>G12*H12</f>
         <v>0.05</v>
       </c>
-      <c r="J12" t="s" s="49">
-        <v>58</v>
-      </c>
-      <c r="K12" s="46">
+      <c r="J12" t="s" s="63">
+        <v>63</v>
+      </c>
+      <c r="K12" s="60">
         <f>G12*J12</f>
         <v>0.05</v>
       </c>
-      <c r="L12" t="s" s="49">
-        <v>58</v>
-      </c>
-      <c r="M12" s="46">
+      <c r="L12" t="s" s="63">
+        <v>63</v>
+      </c>
+      <c r="M12" s="60">
         <f>G12*L12</f>
         <v>0.05</v>
       </c>
-      <c r="N12" t="s" s="49">
-        <v>58</v>
-      </c>
-      <c r="O12" s="46">
+      <c r="N12" t="s" s="63">
+        <v>63</v>
+      </c>
+      <c r="O12" s="60">
         <f>N12*G12</f>
         <v>0.05</v>
       </c>
-      <c r="P12" t="s" s="49">
-        <v>58</v>
-      </c>
-      <c r="Q12" s="50">
+      <c r="P12" t="s" s="63">
+        <v>63</v>
+      </c>
+      <c r="Q12" s="64">
         <f>P12*G12</f>
         <v>0.05</v>
       </c>
+      <c r="R12" t="s" s="75">
+        <v>63</v>
+      </c>
+      <c r="S12" s="60">
+        <f>G12*R12</f>
+        <v>0.05</v>
+      </c>
+      <c r="T12" s="52"/>
+      <c r="U12" s="53"/>
+      <c r="V12" s="52"/>
+      <c r="W12" s="53"/>
+      <c r="X12" s="52"/>
+      <c r="Y12" s="53"/>
+      <c r="Z12" s="52"/>
+      <c r="AA12" s="54"/>
     </row>
     <row r="13" ht="83.1" customHeight="1">
-      <c r="A13" s="31">
+      <c r="A13" s="40">
         <v>10</v>
       </c>
-      <c r="B13" s="32">
+      <c r="B13" s="41">
         <v>45270</v>
       </c>
-      <c r="C13" t="s" s="33">
-        <v>59</v>
-      </c>
-      <c r="D13" t="s" s="34">
-        <v>60</v>
-      </c>
-      <c r="E13" t="s" s="55">
-        <v>61</v>
-      </c>
-      <c r="F13" t="s" s="36">
-        <v>42</v>
-      </c>
-      <c r="G13" t="s" s="52">
-        <v>43</v>
-      </c>
-      <c r="H13" t="s" s="48">
-        <v>21</v>
-      </c>
-      <c r="I13" s="39">
+      <c r="C13" t="s" s="42">
+        <v>64</v>
+      </c>
+      <c r="D13" t="s" s="43">
+        <v>65</v>
+      </c>
+      <c r="E13" t="s" s="76">
+        <v>66</v>
+      </c>
+      <c r="F13" t="s" s="45">
+        <v>47</v>
+      </c>
+      <c r="G13" t="s" s="69">
+        <v>48</v>
+      </c>
+      <c r="H13" t="s" s="62">
+        <v>26</v>
+      </c>
+      <c r="I13" s="48">
         <f>G13*H13</f>
         <v>0.9</v>
       </c>
-      <c r="J13" t="s" s="48">
-        <v>21</v>
-      </c>
-      <c r="K13" s="39">
+      <c r="J13" t="s" s="62">
+        <v>26</v>
+      </c>
+      <c r="K13" s="48">
         <f>G13*J13</f>
         <v>0.9</v>
       </c>
-      <c r="L13" t="s" s="49">
-        <v>33</v>
-      </c>
-      <c r="M13" s="39">
+      <c r="L13" t="s" s="63">
+        <v>38</v>
+      </c>
+      <c r="M13" s="48">
         <f>G13*L13</f>
         <v>0.6</v>
       </c>
-      <c r="N13" t="s" s="48">
-        <v>21</v>
-      </c>
-      <c r="O13" s="39">
+      <c r="N13" t="s" s="62">
+        <v>26</v>
+      </c>
+      <c r="O13" s="48">
         <f>N13*G13</f>
         <v>0.9</v>
       </c>
-      <c r="P13" t="s" s="49">
-        <v>33</v>
-      </c>
-      <c r="Q13" s="40">
+      <c r="P13" t="s" s="63">
+        <v>38</v>
+      </c>
+      <c r="Q13" s="49">
         <f>P13*G13</f>
         <v>0.6</v>
       </c>
+      <c r="R13" t="s" s="77">
+        <v>26</v>
+      </c>
+      <c r="S13" s="48">
+        <f>G13*R13</f>
+        <v>0.9</v>
+      </c>
+      <c r="T13" s="52"/>
+      <c r="U13" s="53"/>
+      <c r="V13" s="52"/>
+      <c r="W13" s="53"/>
+      <c r="X13" s="52"/>
+      <c r="Y13" s="53"/>
+      <c r="Z13" s="52"/>
+      <c r="AA13" s="54"/>
     </row>
     <row r="14" ht="110.1" customHeight="1">
-      <c r="A14" s="31">
+      <c r="A14" s="40">
         <v>11</v>
       </c>
-      <c r="B14" s="41">
+      <c r="B14" s="55">
         <v>45270</v>
       </c>
-      <c r="C14" t="s" s="42">
-        <v>62</v>
-      </c>
-      <c r="D14" t="s" s="34">
-        <v>63</v>
-      </c>
-      <c r="E14" t="s" s="55">
-        <v>64</v>
-      </c>
-      <c r="F14" t="s" s="43">
-        <v>37</v>
-      </c>
-      <c r="G14" t="s" s="52">
-        <v>43</v>
-      </c>
-      <c r="H14" t="s" s="47">
-        <v>20</v>
-      </c>
-      <c r="I14" s="46">
+      <c r="C14" t="s" s="56">
+        <v>67</v>
+      </c>
+      <c r="D14" t="s" s="43">
+        <v>68</v>
+      </c>
+      <c r="E14" t="s" s="76">
+        <v>69</v>
+      </c>
+      <c r="F14" t="s" s="57">
+        <v>42</v>
+      </c>
+      <c r="G14" t="s" s="69">
+        <v>48</v>
+      </c>
+      <c r="H14" t="s" s="61">
+        <v>25</v>
+      </c>
+      <c r="I14" s="60">
         <f>G14*H14</f>
         <v>1.2</v>
       </c>
-      <c r="J14" t="s" s="47">
-        <v>20</v>
-      </c>
-      <c r="K14" s="46">
+      <c r="J14" t="s" s="61">
+        <v>25</v>
+      </c>
+      <c r="K14" s="60">
         <f>G14*J14</f>
         <v>1.2</v>
       </c>
-      <c r="L14" t="s" s="48">
-        <v>21</v>
-      </c>
-      <c r="M14" s="46">
+      <c r="L14" t="s" s="62">
+        <v>26</v>
+      </c>
+      <c r="M14" s="60">
         <f>G14*L14</f>
         <v>0.9</v>
       </c>
-      <c r="N14" t="s" s="48">
-        <v>21</v>
-      </c>
-      <c r="O14" s="46">
+      <c r="N14" t="s" s="62">
+        <v>26</v>
+      </c>
+      <c r="O14" s="60">
         <f>N14*G14</f>
         <v>0.9</v>
       </c>
-      <c r="P14" t="s" s="48">
-        <v>21</v>
-      </c>
-      <c r="Q14" s="50">
+      <c r="P14" t="s" s="62">
+        <v>26</v>
+      </c>
+      <c r="Q14" s="64">
         <f>P14*G14</f>
         <v>0.9</v>
       </c>
+      <c r="R14" t="s" s="71">
+        <v>25</v>
+      </c>
+      <c r="S14" s="60">
+        <f>G14*R14</f>
+        <v>1.2</v>
+      </c>
+      <c r="T14" s="52"/>
+      <c r="U14" s="53"/>
+      <c r="V14" s="52"/>
+      <c r="W14" s="53"/>
+      <c r="X14" s="52"/>
+      <c r="Y14" s="53"/>
+      <c r="Z14" s="52"/>
+      <c r="AA14" s="54"/>
     </row>
     <row r="15" ht="68.2" customHeight="1">
-      <c r="A15" s="31">
+      <c r="A15" s="40">
         <v>12</v>
       </c>
-      <c r="B15" s="32">
+      <c r="B15" s="41">
         <v>45270</v>
       </c>
-      <c r="C15" t="s" s="33">
-        <v>65</v>
-      </c>
-      <c r="D15" t="s" s="34">
-        <v>66</v>
-      </c>
-      <c r="E15" t="s" s="35">
-        <v>67</v>
-      </c>
-      <c r="F15" t="s" s="36">
-        <v>25</v>
-      </c>
-      <c r="G15" t="s" s="37">
-        <v>26</v>
-      </c>
-      <c r="H15" t="s" s="45">
-        <v>32</v>
-      </c>
-      <c r="I15" s="39">
+      <c r="C15" t="s" s="42">
+        <v>70</v>
+      </c>
+      <c r="D15" t="s" s="43">
+        <v>71</v>
+      </c>
+      <c r="E15" t="s" s="44">
+        <v>72</v>
+      </c>
+      <c r="F15" t="s" s="45">
+        <v>30</v>
+      </c>
+      <c r="G15" t="s" s="46">
+        <v>31</v>
+      </c>
+      <c r="H15" t="s" s="59">
+        <v>37</v>
+      </c>
+      <c r="I15" s="48">
         <f>G15*H15</f>
         <v>2.4</v>
       </c>
-      <c r="J15" t="s" s="47">
-        <v>20</v>
-      </c>
-      <c r="K15" s="39">
+      <c r="J15" t="s" s="61">
+        <v>25</v>
+      </c>
+      <c r="K15" s="48">
         <f>G15*J15</f>
         <v>1.6</v>
       </c>
-      <c r="L15" t="s" s="47">
-        <v>20</v>
-      </c>
-      <c r="M15" s="39">
+      <c r="L15" t="s" s="61">
+        <v>25</v>
+      </c>
+      <c r="M15" s="48">
         <f>G15*L15</f>
         <v>1.6</v>
       </c>
-      <c r="N15" t="s" s="47">
-        <v>20</v>
-      </c>
-      <c r="O15" s="39">
+      <c r="N15" t="s" s="61">
+        <v>25</v>
+      </c>
+      <c r="O15" s="48">
         <f>N15*G15</f>
         <v>1.6</v>
       </c>
-      <c r="P15" t="s" s="48">
-        <v>21</v>
-      </c>
-      <c r="Q15" s="40">
+      <c r="P15" t="s" s="62">
+        <v>26</v>
+      </c>
+      <c r="Q15" s="49">
         <f>P15*G15</f>
         <v>1.2</v>
       </c>
+      <c r="R15" t="s" s="77">
+        <v>26</v>
+      </c>
+      <c r="S15" s="48">
+        <f>G15*R15</f>
+        <v>1.2</v>
+      </c>
+      <c r="T15" s="52"/>
+      <c r="U15" s="53"/>
+      <c r="V15" s="52"/>
+      <c r="W15" s="53"/>
+      <c r="X15" s="52"/>
+      <c r="Y15" s="53"/>
+      <c r="Z15" s="52"/>
+      <c r="AA15" s="54"/>
     </row>
     <row r="16" ht="92.2" customHeight="1">
-      <c r="A16" s="31">
+      <c r="A16" s="40">
         <v>13</v>
       </c>
-      <c r="B16" s="41">
+      <c r="B16" s="55">
         <v>45271</v>
       </c>
-      <c r="C16" t="s" s="42">
-        <v>68</v>
-      </c>
-      <c r="D16" t="s" s="34">
-        <v>69</v>
-      </c>
-      <c r="E16" t="s" s="35">
-        <v>70</v>
-      </c>
-      <c r="F16" t="s" s="43">
-        <v>42</v>
-      </c>
-      <c r="G16" t="s" s="37">
-        <v>26</v>
-      </c>
-      <c r="H16" t="s" s="56">
-        <v>71</v>
-      </c>
-      <c r="I16" s="46">
+      <c r="C16" t="s" s="56">
+        <v>73</v>
+      </c>
+      <c r="D16" t="s" s="43">
+        <v>74</v>
+      </c>
+      <c r="E16" t="s" s="44">
+        <v>75</v>
+      </c>
+      <c r="F16" t="s" s="57">
+        <v>47</v>
+      </c>
+      <c r="G16" t="s" s="46">
+        <v>31</v>
+      </c>
+      <c r="H16" t="s" s="78">
+        <v>76</v>
+      </c>
+      <c r="I16" s="60">
         <f>G16*H16</f>
         <v>2.8</v>
       </c>
-      <c r="J16" t="s" s="45">
-        <v>32</v>
-      </c>
-      <c r="K16" s="46">
+      <c r="J16" t="s" s="59">
+        <v>37</v>
+      </c>
+      <c r="K16" s="60">
         <f>G16*J16</f>
         <v>2.4</v>
       </c>
-      <c r="L16" t="s" s="47">
-        <v>20</v>
-      </c>
-      <c r="M16" s="46">
+      <c r="L16" t="s" s="61">
+        <v>25</v>
+      </c>
+      <c r="M16" s="60">
         <f>G16*L16</f>
         <v>1.6</v>
       </c>
-      <c r="N16" t="s" s="45">
-        <v>32</v>
-      </c>
-      <c r="O16" s="46">
+      <c r="N16" t="s" s="59">
+        <v>37</v>
+      </c>
+      <c r="O16" s="60">
         <f>N16*G16</f>
         <v>2.4</v>
       </c>
-      <c r="P16" t="s" s="47">
-        <v>20</v>
-      </c>
-      <c r="Q16" s="50">
+      <c r="P16" t="s" s="61">
+        <v>25</v>
+      </c>
+      <c r="Q16" s="64">
         <f>P16*G16</f>
         <v>1.6</v>
       </c>
+      <c r="R16" t="s" s="71">
+        <v>25</v>
+      </c>
+      <c r="S16" s="60">
+        <f>G16*R16</f>
+        <v>1.6</v>
+      </c>
+      <c r="T16" s="52"/>
+      <c r="U16" s="53"/>
+      <c r="V16" s="52"/>
+      <c r="W16" s="53"/>
+      <c r="X16" s="52"/>
+      <c r="Y16" s="53"/>
+      <c r="Z16" s="52"/>
+      <c r="AA16" s="54"/>
     </row>
     <row r="17" ht="92.2" customHeight="1">
-      <c r="A17" s="31">
+      <c r="A17" s="40">
         <v>14</v>
       </c>
-      <c r="B17" s="32">
+      <c r="B17" s="41">
         <v>45271</v>
       </c>
-      <c r="C17" t="s" s="33">
-        <v>72</v>
-      </c>
-      <c r="D17" t="s" s="34">
-        <v>73</v>
-      </c>
-      <c r="E17" t="s" s="35">
-        <v>74</v>
-      </c>
-      <c r="F17" t="s" s="36">
-        <v>42</v>
-      </c>
-      <c r="G17" t="s" s="52">
-        <v>43</v>
-      </c>
-      <c r="H17" t="s" s="45">
-        <v>32</v>
-      </c>
-      <c r="I17" s="39">
+      <c r="C17" t="s" s="42">
+        <v>77</v>
+      </c>
+      <c r="D17" t="s" s="43">
+        <v>78</v>
+      </c>
+      <c r="E17" t="s" s="44">
+        <v>79</v>
+      </c>
+      <c r="F17" t="s" s="45">
+        <v>47</v>
+      </c>
+      <c r="G17" t="s" s="69">
+        <v>48</v>
+      </c>
+      <c r="H17" t="s" s="59">
+        <v>37</v>
+      </c>
+      <c r="I17" s="48">
         <f>G17*H17</f>
         <v>1.8</v>
       </c>
-      <c r="J17" t="s" s="45">
-        <v>32</v>
-      </c>
-      <c r="K17" s="39">
+      <c r="J17" t="s" s="59">
+        <v>37</v>
+      </c>
+      <c r="K17" s="48">
         <f>G17*J17</f>
         <v>1.8</v>
       </c>
-      <c r="L17" t="s" s="47">
-        <v>20</v>
-      </c>
-      <c r="M17" s="39">
+      <c r="L17" t="s" s="61">
+        <v>25</v>
+      </c>
+      <c r="M17" s="48">
         <f>G17*L17</f>
         <v>1.2</v>
       </c>
-      <c r="N17" t="s" s="45">
-        <v>32</v>
-      </c>
-      <c r="O17" s="39">
+      <c r="N17" t="s" s="59">
+        <v>37</v>
+      </c>
+      <c r="O17" s="48">
         <f>N17*G17</f>
         <v>1.8</v>
       </c>
-      <c r="P17" t="s" s="47">
-        <v>20</v>
-      </c>
-      <c r="Q17" s="40">
+      <c r="P17" t="s" s="61">
+        <v>25</v>
+      </c>
+      <c r="Q17" s="49">
         <f>P17*G17</f>
         <v>1.2</v>
       </c>
+      <c r="R17" t="s" s="71">
+        <v>25</v>
+      </c>
+      <c r="S17" s="48">
+        <f>G17*R17</f>
+        <v>1.2</v>
+      </c>
+      <c r="T17" s="52"/>
+      <c r="U17" s="53"/>
+      <c r="V17" s="52"/>
+      <c r="W17" s="53"/>
+      <c r="X17" s="52"/>
+      <c r="Y17" s="53"/>
+      <c r="Z17" s="52"/>
+      <c r="AA17" s="54"/>
     </row>
     <row r="18" ht="68.2" customHeight="1">
-      <c r="A18" s="31">
+      <c r="A18" s="40">
         <v>15</v>
       </c>
-      <c r="B18" s="41">
+      <c r="B18" s="55">
         <v>45271</v>
       </c>
-      <c r="C18" t="s" s="42">
-        <v>75</v>
-      </c>
-      <c r="D18" t="s" s="34">
-        <v>76</v>
-      </c>
-      <c r="E18" t="s" s="35">
-        <v>77</v>
-      </c>
-      <c r="F18" t="s" s="43">
-        <v>78</v>
-      </c>
-      <c r="G18" t="s" s="52">
-        <v>43</v>
-      </c>
-      <c r="H18" t="s" s="45">
-        <v>32</v>
-      </c>
-      <c r="I18" s="46">
+      <c r="C18" t="s" s="56">
+        <v>80</v>
+      </c>
+      <c r="D18" t="s" s="43">
+        <v>81</v>
+      </c>
+      <c r="E18" t="s" s="44">
+        <v>82</v>
+      </c>
+      <c r="F18" t="s" s="57">
+        <v>83</v>
+      </c>
+      <c r="G18" t="s" s="69">
+        <v>48</v>
+      </c>
+      <c r="H18" t="s" s="59">
+        <v>37</v>
+      </c>
+      <c r="I18" s="60">
         <f>G18*H18</f>
         <v>1.8</v>
       </c>
-      <c r="J18" t="s" s="45">
-        <v>32</v>
-      </c>
-      <c r="K18" s="46">
+      <c r="J18" t="s" s="59">
+        <v>37</v>
+      </c>
+      <c r="K18" s="60">
         <f>G18*J18</f>
         <v>1.8</v>
       </c>
-      <c r="L18" t="s" s="45">
-        <v>32</v>
-      </c>
-      <c r="M18" s="46">
+      <c r="L18" t="s" s="59">
+        <v>37</v>
+      </c>
+      <c r="M18" s="60">
         <f>G18*L18</f>
         <v>1.8</v>
       </c>
-      <c r="N18" t="s" s="57">
-        <v>79</v>
-      </c>
-      <c r="O18" s="46">
+      <c r="N18" t="s" s="79">
+        <v>84</v>
+      </c>
+      <c r="O18" s="60">
         <f>N18*G18</f>
         <v>1.5</v>
       </c>
-      <c r="P18" t="s" s="57">
-        <v>79</v>
-      </c>
-      <c r="Q18" s="50">
+      <c r="P18" t="s" s="79">
+        <v>84</v>
+      </c>
+      <c r="Q18" s="64">
         <f>P18*G18</f>
         <v>1.5</v>
       </c>
+      <c r="R18" t="s" s="73">
+        <v>37</v>
+      </c>
+      <c r="S18" s="60">
+        <f>G18*R18</f>
+        <v>1.8</v>
+      </c>
+      <c r="T18" s="52"/>
+      <c r="U18" s="53"/>
+      <c r="V18" s="52"/>
+      <c r="W18" s="53"/>
+      <c r="X18" s="52"/>
+      <c r="Y18" s="53"/>
+      <c r="Z18" s="52"/>
+      <c r="AA18" s="54"/>
     </row>
     <row r="19" ht="56.2" customHeight="1">
-      <c r="A19" s="31">
+      <c r="A19" s="40">
         <v>16</v>
       </c>
-      <c r="B19" s="32">
+      <c r="B19" s="41">
         <v>45272</v>
       </c>
-      <c r="C19" t="s" s="33">
-        <v>80</v>
-      </c>
-      <c r="D19" t="s" s="34">
-        <v>81</v>
-      </c>
-      <c r="E19" t="s" s="35">
-        <v>77</v>
-      </c>
-      <c r="F19" t="s" s="36">
-        <v>78</v>
-      </c>
-      <c r="G19" t="s" s="37">
-        <v>26</v>
-      </c>
-      <c r="H19" t="s" s="49">
-        <v>33</v>
-      </c>
-      <c r="I19" s="39">
+      <c r="C19" t="s" s="42">
+        <v>85</v>
+      </c>
+      <c r="D19" t="s" s="43">
+        <v>86</v>
+      </c>
+      <c r="E19" t="s" s="44">
+        <v>82</v>
+      </c>
+      <c r="F19" t="s" s="45">
+        <v>83</v>
+      </c>
+      <c r="G19" t="s" s="46">
+        <v>31</v>
+      </c>
+      <c r="H19" t="s" s="63">
+        <v>38</v>
+      </c>
+      <c r="I19" s="48">
         <f>G19*H19</f>
         <v>0.8</v>
       </c>
-      <c r="J19" t="s" s="49">
-        <v>33</v>
-      </c>
-      <c r="K19" s="39">
+      <c r="J19" t="s" s="63">
+        <v>38</v>
+      </c>
+      <c r="K19" s="48">
         <f>G19*J19</f>
         <v>0.8</v>
       </c>
-      <c r="L19" t="s" s="49">
-        <v>33</v>
-      </c>
-      <c r="M19" s="39">
+      <c r="L19" t="s" s="63">
+        <v>38</v>
+      </c>
+      <c r="M19" s="48">
         <f>G19*L19</f>
         <v>0.8</v>
       </c>
-      <c r="N19" t="s" s="48">
-        <v>21</v>
-      </c>
-      <c r="O19" s="39">
+      <c r="N19" t="s" s="62">
+        <v>26</v>
+      </c>
+      <c r="O19" s="48">
         <f>N19*G19</f>
         <v>1.2</v>
       </c>
-      <c r="P19" t="s" s="48">
-        <v>21</v>
-      </c>
-      <c r="Q19" s="40">
+      <c r="P19" t="s" s="62">
+        <v>26</v>
+      </c>
+      <c r="Q19" s="49">
         <f>P19*G19</f>
         <v>1.2</v>
       </c>
+      <c r="R19" t="s" s="75">
+        <v>38</v>
+      </c>
+      <c r="S19" s="48">
+        <f>G19*R19</f>
+        <v>0.8</v>
+      </c>
+      <c r="T19" s="52"/>
+      <c r="U19" s="53"/>
+      <c r="V19" s="52"/>
+      <c r="W19" s="53"/>
+      <c r="X19" s="52"/>
+      <c r="Y19" s="53"/>
+      <c r="Z19" s="52"/>
+      <c r="AA19" s="54"/>
     </row>
     <row r="20" ht="104.2" customHeight="1">
-      <c r="A20" s="31">
+      <c r="A20" s="40">
         <v>17</v>
       </c>
-      <c r="B20" s="41">
+      <c r="B20" s="55">
         <v>45273</v>
       </c>
-      <c r="C20" t="s" s="42">
-        <v>82</v>
-      </c>
-      <c r="D20" t="s" s="34">
-        <v>83</v>
-      </c>
-      <c r="E20" t="s" s="35">
-        <v>84</v>
-      </c>
-      <c r="F20" t="s" s="43">
-        <v>42</v>
-      </c>
-      <c r="G20" t="s" s="44">
-        <v>31</v>
-      </c>
-      <c r="H20" t="s" s="48">
-        <v>21</v>
-      </c>
-      <c r="I20" s="46">
+      <c r="C20" t="s" s="56">
+        <v>87</v>
+      </c>
+      <c r="D20" t="s" s="43">
+        <v>88</v>
+      </c>
+      <c r="E20" t="s" s="44">
+        <v>89</v>
+      </c>
+      <c r="F20" t="s" s="57">
+        <v>47</v>
+      </c>
+      <c r="G20" t="s" s="58">
+        <v>36</v>
+      </c>
+      <c r="H20" t="s" s="62">
+        <v>26</v>
+      </c>
+      <c r="I20" s="60">
         <f>G20*H20</f>
         <v>1.5</v>
       </c>
-      <c r="J20" t="s" s="48">
-        <v>21</v>
-      </c>
-      <c r="K20" s="46">
+      <c r="J20" t="s" s="62">
+        <v>26</v>
+      </c>
+      <c r="K20" s="60">
         <f>G20*J20</f>
         <v>1.5</v>
       </c>
-      <c r="L20" t="s" s="48">
-        <v>21</v>
-      </c>
-      <c r="M20" s="46">
+      <c r="L20" t="s" s="62">
+        <v>26</v>
+      </c>
+      <c r="M20" s="60">
         <f>G20*L20</f>
         <v>1.5</v>
       </c>
-      <c r="N20" t="s" s="49">
-        <v>33</v>
-      </c>
-      <c r="O20" s="46">
+      <c r="N20" t="s" s="63">
+        <v>38</v>
+      </c>
+      <c r="O20" s="60">
         <f>N20*G20</f>
         <v>1</v>
       </c>
-      <c r="P20" t="s" s="38">
-        <v>27</v>
-      </c>
-      <c r="Q20" s="50">
+      <c r="P20" t="s" s="47">
+        <v>32</v>
+      </c>
+      <c r="Q20" s="64">
         <f>P20*G20</f>
         <v>0.5</v>
       </c>
+      <c r="R20" t="s" s="77">
+        <v>26</v>
+      </c>
+      <c r="S20" s="60">
+        <f>G20*R20</f>
+        <v>1.5</v>
+      </c>
+      <c r="T20" s="52"/>
+      <c r="U20" s="53"/>
+      <c r="V20" s="52"/>
+      <c r="W20" s="53"/>
+      <c r="X20" s="52"/>
+      <c r="Y20" s="53"/>
+      <c r="Z20" s="52"/>
+      <c r="AA20" s="54"/>
     </row>
     <row r="21" ht="80.2" customHeight="1">
-      <c r="A21" s="58">
+      <c r="A21" s="80">
         <v>18</v>
       </c>
-      <c r="B21" s="59">
+      <c r="B21" s="81">
         <v>45273</v>
       </c>
-      <c r="C21" t="s" s="60">
-        <v>85</v>
-      </c>
-      <c r="D21" t="s" s="61">
-        <v>86</v>
-      </c>
-      <c r="E21" t="s" s="62">
-        <v>87</v>
-      </c>
-      <c r="F21" t="s" s="63">
-        <v>25</v>
-      </c>
-      <c r="G21" t="s" s="64">
-        <v>38</v>
-      </c>
-      <c r="H21" t="s" s="65">
-        <v>79</v>
-      </c>
-      <c r="I21" s="66">
+      <c r="C21" t="s" s="82">
+        <v>90</v>
+      </c>
+      <c r="D21" t="s" s="83">
+        <v>91</v>
+      </c>
+      <c r="E21" t="s" s="84">
+        <v>92</v>
+      </c>
+      <c r="F21" t="s" s="85">
+        <v>30</v>
+      </c>
+      <c r="G21" t="s" s="86">
+        <v>43</v>
+      </c>
+      <c r="H21" t="s" s="87">
+        <v>84</v>
+      </c>
+      <c r="I21" s="88">
         <f>G21*H21</f>
         <v>1</v>
       </c>
-      <c r="J21" t="s" s="65">
-        <v>79</v>
-      </c>
-      <c r="K21" s="66">
+      <c r="J21" t="s" s="87">
+        <v>84</v>
+      </c>
+      <c r="K21" s="88">
         <f>G21*J21</f>
         <v>1</v>
       </c>
-      <c r="L21" t="s" s="67">
-        <v>20</v>
-      </c>
-      <c r="M21" s="66">
+      <c r="L21" t="s" s="89">
+        <v>25</v>
+      </c>
+      <c r="M21" s="88">
         <f>G21*L21</f>
         <v>0.8</v>
       </c>
-      <c r="N21" t="s" s="67">
-        <v>20</v>
-      </c>
-      <c r="O21" s="66">
+      <c r="N21" t="s" s="89">
+        <v>25</v>
+      </c>
+      <c r="O21" s="88">
         <f>N21*G21</f>
         <v>0.8</v>
       </c>
-      <c r="P21" t="s" s="67">
-        <v>20</v>
-      </c>
-      <c r="Q21" s="68">
+      <c r="P21" t="s" s="89">
+        <v>25</v>
+      </c>
+      <c r="Q21" s="90">
         <f>P21*G21</f>
         <v>0.8</v>
       </c>
+      <c r="R21" t="s" s="91">
+        <v>84</v>
+      </c>
+      <c r="S21" s="88">
+        <f>G21*R21</f>
+        <v>1</v>
+      </c>
+      <c r="T21" s="92"/>
+      <c r="U21" s="93"/>
+      <c r="V21" s="92"/>
+      <c r="W21" s="93"/>
+      <c r="X21" s="92"/>
+      <c r="Y21" s="93"/>
+      <c r="Z21" s="92"/>
+      <c r="AA21" s="94"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="A1:Q1"/>
+  <mergeCells count="11">
+    <mergeCell ref="A1:AA1"/>
     <mergeCell ref="H2:I2"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="L2:M2"/>
     <mergeCell ref="N2:O2"/>
     <mergeCell ref="P2:Q2"/>
+    <mergeCell ref="R2:S2"/>
+    <mergeCell ref="T2:U2"/>
+    <mergeCell ref="V2:W2"/>
+    <mergeCell ref="X2:Y2"/>
+    <mergeCell ref="Z2:AA2"/>
   </mergeCells>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="72" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>